<commit_message>
Update Ofertas de Disciplinas- UFMG PPGCC.xlsx
</commit_message>
<xml_diff>
--- a/Files/Disciplinas/Ofertas de Disciplinas- UFMG PPGCC.xlsx
+++ b/Files/Disciplinas/Ofertas de Disciplinas- UFMG PPGCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\UFMG\MiscDocs_PPGCC\Files\Disciplinas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB084E9A-131F-4079-B532-475B52BBCA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE8D5D4-A0EB-43A4-8463-740D9B3AA8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="980" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025.1 horários JV" sheetId="28" r:id="rId1"/>
@@ -11062,7 +11062,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -21189,8 +21189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFD6A5D-4252-4C92-9D84-040616A2AE3A}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21795,7 +21795,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="126">
-        <v>45727</v>
+        <v>45729</v>
       </c>
       <c r="D14" s="122">
         <v>18</v>

</xml_diff>